<commit_message>
10.03.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/March/All Details/09.03.2020/MC Bank Statement March 2020.xlsx
+++ b/2020/March/All Details/09.03.2020/MC Bank Statement March 2020.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>Date: 09.03.2020</t>
+  </si>
+  <si>
+    <t>Today Sales</t>
+  </si>
+  <si>
+    <t>C.Stock</t>
+  </si>
+  <si>
+    <t>O.Stock</t>
   </si>
 </sst>
 </file>
@@ -651,7 +660,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -768,19 +777,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1010,8 +1006,8 @@
     <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
@@ -1022,12 +1018,12 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -1036,15 +1032,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1262,9 +1258,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1272,9 +1265,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1293,27 +1283,12 @@
     <xf numFmtId="2" fontId="5" fillId="36" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1341,10 +1316,10 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="35" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1379,7 +1354,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1389,7 +1364,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="35" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1440,15 +1415,15 @@
     <xf numFmtId="0" fontId="4" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1458,14 +1433,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -1558,7 +1557,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1570,7 +1569,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1593,14 +1592,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1927,21 +1926,21 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="20.25">
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="134" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1">
       <c r="A3" s="59"/>
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="B4" s="60" t="s">
@@ -1956,7 +1955,7 @@
       <c r="E4" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="134" t="s">
+      <c r="F4" s="127" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1970,7 +1969,7 @@
       <c r="D5" s="63">
         <v>0</v>
       </c>
-      <c r="E5" s="133">
+      <c r="E5" s="126">
         <f>C5-D5</f>
         <v>3000</v>
       </c>
@@ -2016,7 +2015,7 @@
       <c r="C8" s="63">
         <v>282000</v>
       </c>
-      <c r="D8" s="87">
+      <c r="D8" s="85">
         <v>295000</v>
       </c>
       <c r="E8" s="66">
@@ -2029,20 +2028,20 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="59"/>
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="87">
+      <c r="C9" s="85">
         <v>300000</v>
       </c>
-      <c r="D9" s="87">
+      <c r="D9" s="85">
         <v>300000</v>
       </c>
-      <c r="E9" s="139">
+      <c r="E9" s="132">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="F9" s="138" t="s">
+      <c r="F9" s="131" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="2"/>
@@ -2056,7 +2055,7 @@
       <c r="C10" s="67">
         <v>100000</v>
       </c>
-      <c r="D10" s="137">
+      <c r="D10" s="130">
         <v>100000</v>
       </c>
       <c r="E10" s="66">
@@ -2094,14 +2093,14 @@
       <c r="C12" s="63">
         <v>410000</v>
       </c>
-      <c r="D12" s="135">
+      <c r="D12" s="128">
         <v>450000</v>
       </c>
       <c r="E12" s="66">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="F12" s="136" t="s">
+      <c r="F12" s="129" t="s">
         <v>37</v>
       </c>
       <c r="G12" s="68"/>
@@ -2115,14 +2114,14 @@
       <c r="C13" s="63">
         <v>350000</v>
       </c>
-      <c r="D13" s="135">
+      <c r="D13" s="128">
         <v>350000</v>
       </c>
       <c r="E13" s="66">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="F13" s="136" t="s">
+      <c r="F13" s="129" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="2"/>
@@ -2136,14 +2135,14 @@
       <c r="C14" s="63">
         <v>200000</v>
       </c>
-      <c r="D14" s="135">
+      <c r="D14" s="128">
         <v>200000</v>
       </c>
       <c r="E14" s="66">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="F14" s="136" t="s">
+      <c r="F14" s="129" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="2"/>
@@ -2157,7 +2156,7 @@
       <c r="C15" s="63">
         <v>0</v>
       </c>
-      <c r="D15" s="135">
+      <c r="D15" s="128">
         <v>0</v>
       </c>
       <c r="E15" s="66">
@@ -2179,14 +2178,14 @@
       <c r="C16" s="63">
         <v>400000</v>
       </c>
-      <c r="D16" s="135">
+      <c r="D16" s="128">
         <v>400000</v>
       </c>
       <c r="E16" s="66">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="F16" s="136" t="s">
+      <c r="F16" s="129" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="57"/>
@@ -2226,7 +2225,7 @@
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="F18" s="136" t="s">
+      <c r="F18" s="129" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="68"/>
@@ -2240,7 +2239,7 @@
       <c r="C19" s="63">
         <v>110000</v>
       </c>
-      <c r="D19" s="87">
+      <c r="D19" s="85">
         <v>110000</v>
       </c>
       <c r="E19" s="66">
@@ -2278,7 +2277,7 @@
       <c r="C21" s="63">
         <v>50000</v>
       </c>
-      <c r="D21" s="87">
+      <c r="D21" s="85">
         <v>400000</v>
       </c>
       <c r="E21" s="66">
@@ -3061,7 +3060,7 @@
   <dimension ref="A1:AK222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" customHeight="1"/>
@@ -3077,7 +3076,7 @@
     <col min="9" max="9" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -3085,24 +3084,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="26.25">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="145"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="138"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="148"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="141"/>
       <c r="F2" s="5"/>
       <c r="G2" s="13"/>
       <c r="H2" s="2"/>
@@ -3137,11 +3136,11 @@
       <c r="AK2" s="8"/>
     </row>
     <row r="3" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A3" s="100"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="101"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="5"/>
       <c r="G3" s="11"/>
       <c r="I3" s="2"/>
@@ -3181,25 +3180,25 @@
       <c r="B4" s="28">
         <v>6500000</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="119" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="102">
+      <c r="E4" s="95">
         <v>4377421.1099999994</v>
       </c>
-      <c r="F4" s="131">
+      <c r="F4" s="124">
         <v>2233</v>
       </c>
-      <c r="G4" s="95"/>
+      <c r="G4" s="88"/>
       <c r="H4" s="68"/>
       <c r="I4" s="76"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
@@ -3230,23 +3229,31 @@
       <c r="B5" s="28">
         <v>69770.390000000014</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="119" t="s">
+      <c r="C5" s="78"/>
+      <c r="D5" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="102">
+      <c r="E5" s="95">
         <v>3000</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="147" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="148" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="149" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="149" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
@@ -3278,20 +3285,29 @@
         <f>B4+B5</f>
         <v>6569770.3899999997</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="99" t="s">
+      <c r="C6" s="77"/>
+      <c r="D6" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="103">
+      <c r="E6" s="96">
         <v>300000</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="49"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="150">
+        <v>4505494</v>
+      </c>
+      <c r="J6" s="150">
+        <v>299695</v>
+      </c>
+      <c r="K6" s="152">
+        <f>I6-J6</f>
+        <v>4205799</v>
+      </c>
+      <c r="L6" s="150" t="s">
+        <v>45</v>
+      </c>
       <c r="M6" s="49"/>
       <c r="N6" s="49"/>
       <c r="O6" s="49"/>
@@ -3324,22 +3340,25 @@
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="19"/>
-      <c r="D7" s="119" t="s">
+      <c r="D7" s="112" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="39">
         <v>1958567</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="82"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="150">
+        <f>K6</f>
+        <v>4205799</v>
+      </c>
+      <c r="J7" s="150"/>
+      <c r="K7" s="152"/>
+      <c r="L7" s="150"/>
       <c r="M7" s="49"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
@@ -3371,15 +3390,18 @@
         <v>8280</v>
       </c>
       <c r="C8" s="19"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="102"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="95"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="82"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="150">
+        <f>K7</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="150"/>
+      <c r="K8" s="152"/>
+      <c r="L8" s="150"/>
       <c r="M8" s="49"/>
       <c r="N8" s="49"/>
       <c r="O8" s="49"/>
@@ -3407,26 +3429,28 @@
       <c r="AK8" s="8"/>
     </row>
     <row r="9" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A9" s="132"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="29"/>
       <c r="C9" s="19"/>
       <c r="D9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="102">
+      <c r="E9" s="95">
         <v>-77497.719999999739</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="130" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="94"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="49"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="151">
+        <f>K8</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="150"/>
+      <c r="K9" s="152"/>
+      <c r="L9" s="151"/>
       <c r="M9" s="49"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
@@ -3459,17 +3483,21 @@
         <v>61490.390000000014</v>
       </c>
       <c r="C10" s="19"/>
-      <c r="D10" s="119"/>
+      <c r="D10" s="112"/>
       <c r="E10" s="39"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="80"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="53"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="83"/>
+      <c r="I10" s="151">
+        <f>K9</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="150"/>
+      <c r="K10" s="152"/>
+      <c r="L10" s="151"/>
       <c r="M10" s="49"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
@@ -3502,15 +3530,15 @@
       <c r="D11" s="18"/>
       <c r="E11" s="39"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
       <c r="M11" s="49"/>
-      <c r="N11" s="82"/>
-      <c r="O11" s="82"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -3545,7 +3573,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="16"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="93"/>
+      <c r="I12" s="87"/>
       <c r="J12" s="8"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
@@ -3592,7 +3620,7 @@
         <v>6561490.3899999997</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="87">
+      <c r="G13" s="85">
         <f>B13-E13</f>
         <v>0</v>
       </c>
@@ -3628,13 +3656,13 @@
       <c r="AK13" s="8"/>
     </row>
     <row r="14" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A14" s="104"/>
+      <c r="A14" s="97"/>
       <c r="B14" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="44"/>
-      <c r="E14" s="105"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="5"/>
       <c r="G14" s="11"/>
       <c r="H14" s="15"/>
@@ -3669,13 +3697,13 @@
       <c r="AK14" s="8"/>
     </row>
     <row r="15" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A15" s="149" t="s">
+      <c r="A15" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="150"/>
-      <c r="C15" s="150"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="151"/>
+      <c r="B15" s="143"/>
+      <c r="C15" s="143"/>
+      <c r="D15" s="143"/>
+      <c r="E15" s="144"/>
       <c r="F15" s="5"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -3710,22 +3738,22 @@
       <c r="AK15" s="8"/>
     </row>
     <row r="16" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="84">
+      <c r="B16" s="82">
         <v>171144</v>
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="107">
+      <c r="E16" s="100">
         <v>196955</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="96"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="89"/>
       <c r="I16" s="10"/>
       <c r="J16" s="8"/>
       <c r="K16" s="49"/>
@@ -3757,21 +3785,21 @@
       <c r="AK16" s="8"/>
     </row>
     <row r="17" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="85">
+      <c r="B17" s="83">
         <v>20000</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="108">
+      <c r="E17" s="101">
         <v>443675</v>
       </c>
-      <c r="G17" s="97"/>
-      <c r="H17" s="96"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="89"/>
       <c r="I17" s="10"/>
       <c r="J17" s="8"/>
       <c r="K17" s="49"/>
@@ -3803,21 +3831,21 @@
       <c r="AK17" s="8"/>
     </row>
     <row r="18" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="85">
+      <c r="B18" s="83">
         <v>57000</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="110">
+      <c r="E18" s="103">
         <v>306950</v>
       </c>
-      <c r="G18" s="97"/>
-      <c r="H18" s="96"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="89"/>
       <c r="I18" s="52"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -3849,21 +3877,21 @@
       <c r="AK18" s="8"/>
     </row>
     <row r="19" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A19" s="111" t="s">
+      <c r="A19" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="86">
+      <c r="B19" s="84">
         <v>67000</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="110">
+      <c r="E19" s="103">
         <v>241150</v>
       </c>
-      <c r="G19" s="97"/>
-      <c r="H19" s="96"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="89"/>
       <c r="I19" s="12"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -3895,21 +3923,21 @@
       <c r="AK19" s="8"/>
     </row>
     <row r="20" spans="1:37" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A20" s="125" t="s">
+      <c r="A20" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="126">
+      <c r="B20" s="119">
         <v>100000</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="128" t="s">
+      <c r="C20" s="120"/>
+      <c r="D20" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="129">
+      <c r="E20" s="122">
         <v>106000</v>
       </c>
-      <c r="G20" s="97"/>
-      <c r="H20" s="98"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="91"/>
       <c r="I20" s="52"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -3941,11 +3969,11 @@
       <c r="AK20" s="8"/>
     </row>
     <row r="21" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A21" s="120"/>
-      <c r="B21" s="121"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="124"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="117"/>
       <c r="G21" s="48"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -3979,11 +4007,11 @@
       <c r="AK21" s="8"/>
     </row>
     <row r="22" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A22" s="111"/>
-      <c r="B22" s="86"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="31"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="110"/>
+      <c r="E22" s="103"/>
       <c r="G22" s="53"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -4017,11 +4045,11 @@
       <c r="AK22" s="8"/>
     </row>
     <row r="23" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A23" s="106"/>
-      <c r="B23" s="86"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="84"/>
       <c r="C23" s="31"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="105"/>
       <c r="G23" s="53"/>
       <c r="H23" s="8"/>
       <c r="I23" s="15"/>
@@ -4055,11 +4083,11 @@
       <c r="AK23" s="8"/>
     </row>
     <row r="24" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A24" s="111"/>
-      <c r="B24" s="86"/>
+      <c r="A24" s="104"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="31"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="110"/>
+      <c r="E24" s="103"/>
       <c r="G24" s="54"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -4093,11 +4121,11 @@
       <c r="AK24" s="8"/>
     </row>
     <row r="25" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A25" s="109"/>
-      <c r="B25" s="85"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="83"/>
       <c r="C25" s="31"/>
       <c r="D25" s="33"/>
-      <c r="E25" s="108"/>
+      <c r="E25" s="101"/>
       <c r="G25" s="53"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -4131,11 +4159,11 @@
       <c r="AK25" s="8"/>
     </row>
     <row r="26" spans="1:37" ht="21.75" customHeight="1">
-      <c r="A26" s="113"/>
-      <c r="B26" s="86"/>
+      <c r="A26" s="106"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="31"/>
       <c r="D26" s="32"/>
-      <c r="E26" s="110"/>
+      <c r="E26" s="103"/>
       <c r="F26" s="7"/>
       <c r="G26" s="54"/>
       <c r="H26" s="48"/>
@@ -4170,11 +4198,11 @@
       <c r="AK26" s="8"/>
     </row>
     <row r="27" spans="1:37" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A27" s="114"/>
-      <c r="B27" s="115"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="117"/>
-      <c r="E27" s="118"/>
+      <c r="A27" s="107"/>
+      <c r="B27" s="108"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="111"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>

</xml_diff>